<commit_message>
Updated Burndown for sprint 2
</commit_message>
<xml_diff>
--- a/Burndown Chart.xlsx
+++ b/Burndown Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Agile Group Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\Agile Group Work\Git Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4AF400E8-0879-4B56-9257-4E4F0E8FFCE9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{35F25AB7-E814-49DD-BD7F-ED922A2DD659}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7515" xr2:uid="{99E84065-7492-4FA8-B857-18F92DE39364}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Est. Time per Task</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Modify Logo</t>
   </si>
   <si>
-    <t>Investigate CI in general</t>
-  </si>
-  <si>
     <t>Set up Physical board</t>
   </si>
   <si>
@@ -60,12 +57,6 @@
     <t>Set up trello</t>
   </si>
   <si>
-    <t>Set up group</t>
-  </si>
-  <si>
-    <t>Set up whatsapp group</t>
-  </si>
-  <si>
     <t>Create Burndown chart for last week</t>
   </si>
   <si>
@@ -75,17 +66,68 @@
     <t>Sprint 1 (3 Members)</t>
   </si>
   <si>
-    <t>Timeslot (20 mins each over 2 hours)</t>
-  </si>
-  <si>
     <t>Set up Burndown data file</t>
+  </si>
+  <si>
+    <t>Set up IBM Cloud</t>
+  </si>
+  <si>
+    <t>Investigate CI in general Eoin</t>
+  </si>
+  <si>
+    <t>Investigate CI in general Danial</t>
+  </si>
+  <si>
+    <t>Investigate CI in general Eoghan</t>
+  </si>
+  <si>
+    <t>Investigate CI in general James</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Select Group Name</t>
+  </si>
+  <si>
+    <t>Select Group Logo</t>
+  </si>
+  <si>
+    <t>Create whatsapp group</t>
+  </si>
+  <si>
+    <t>aquire sticky notes</t>
+  </si>
+  <si>
+    <t>Discuss project plan</t>
+  </si>
+  <si>
+    <t>Gather data for burndown chart</t>
+  </si>
+  <si>
+    <t>Create google doc for project dictionary</t>
+  </si>
+  <si>
+    <t>Share dictionary</t>
+  </si>
+  <si>
+    <t>Add to dictionary</t>
+  </si>
+  <si>
+    <t>At this scale the management of the agile processes takes as much time as the work itself</t>
+  </si>
+  <si>
+    <t>Add group members to whatsapp group</t>
+  </si>
+  <si>
+    <t>Review Sprint 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +164,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -143,12 +191,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,6 +327,9 @@
                 <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -288,21 +340,24 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>150</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -585,10 +640,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$H$4:$H$9</c:f>
+              <c:f>Sheet1!$H$4:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -606,16 +661,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$4:$I$9</c:f>
+              <c:f>Sheet1!$I$4:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>290</c:v>
                 </c:pt>
@@ -632,6 +690,9 @@
                   <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
@@ -1942,13 +2003,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>610659</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>74083</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1978,13 +2039,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>4233</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>42333</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>21166</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2310,10 +2371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09841128-4773-46A7-8228-697AE377A9E7}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2328,7 +2389,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2350,13 +2411,13 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
         <v>2</v>
@@ -2364,16 +2425,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>150</v>
+        <v>280</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -2384,16 +2445,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5">
-        <v>110</v>
+        <v>220</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -2404,7 +2465,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>30</v>
@@ -2413,7 +2474,7 @@
         <v>3</v>
       </c>
       <c r="F6">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -2424,7 +2485,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1">
         <v>30</v>
@@ -2433,7 +2494,7 @@
         <v>4</v>
       </c>
       <c r="F7">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="H7">
         <v>4</v>
@@ -2444,7 +2505,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
         <v>10</v>
@@ -2453,7 +2514,7 @@
         <v>5</v>
       </c>
       <c r="F8">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="H8">
         <v>5</v>
@@ -2464,7 +2525,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>30</v>
@@ -2473,7 +2534,7 @@
         <v>6</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="H9">
         <v>6</v>
@@ -2483,47 +2544,170 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <f>SUM(B4:B9)</f>
-        <v>150</v>
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>30</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>0</v>
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="2">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="B13" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>240</v>
+        <v>25</v>
+      </c>
+      <c r="B14" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4">
+      <c r="B15">
+        <f>SUM(B4:B14)</f>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <f>SUM(B13:B15)</f>
-        <v>290</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>